<commit_message>
fix fungsi halaman admin/jurusan
</commit_message>
<xml_diff>
--- a/public/files/templates/Template_Jurusan.xlsx
+++ b/public/files/templates/Template_Jurusan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP Victus\Desktop\Asesmen-CPL\public\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0100B61A-D06F-44FE-A54E-FEC9CE427139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DD9B3D-507F-447B-9D44-36A4CCD224CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D9A2ADB2-9425-4ACC-A189-E65F0FB9DDFF}"/>
   </bookViews>
@@ -36,32 +36,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>HP Victus</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{43E9074E-DD85-481E-8E52-06D49172004F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Golongan diisi dengan "Rekayasa" atau "Nonrekayasa" tanpa tanda petik. Pilih melalui dropdown.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Nama Jurusan</t>
   </si>
@@ -74,12 +50,15 @@
   <si>
     <t>Nonrekayasa</t>
   </si>
+  <si>
+    <t>Nomor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,23 +74,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -119,17 +97,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,8 +472,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87B55FE-2CA4-40D3-92C6-D5BE80C2A313}">
-  <dimension ref="A1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87B55FE-2CA4-40D3-92C6-D5BE80C2A313}">
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -473,47 +481,129 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="5" width="8.88671875" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" hidden="1"/>
+    <col min="1" max="1" width="10.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="40.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="17" x14ac:dyDescent="0.3"/>
-    <row r="18" x14ac:dyDescent="0.3"/>
-    <row r="19" x14ac:dyDescent="0.3"/>
-    <row r="20" x14ac:dyDescent="0.3"/>
-    <row r="21" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="6"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="mbvt6TMQcZndEuQ3IcFoXJwWkx7DJc+BKHCrBtkK01e4aVZJFnCPoI9Fhy4sHLz0QbmWZAHZURn+VL012S6a1w==" saltValue="anxGBnZzuXl70grudyiLgQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="8hPtsrzMlrmg7J48Z7hD9ltbfeuAefqpaffc8dyh1yL8DJSy7CEYEAnSnEA2oJrXwy2rMkMNbBOF41nPoOJOMg==" saltValue="04SIF2SwOgBnmza78ghjEg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
-    <protectedRange sqref="A2:B21" name="Range1"/>
+    <protectedRange sqref="A2:C21" name="Range1"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -521,7 +611,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B21</xm:sqref>
+          <xm:sqref>C2:C21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>